<commit_message>
adjusting results analysis plots
</commit_message>
<xml_diff>
--- a/resources/test_hmm_computations.xlsx
+++ b/resources/test_hmm_computations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomyaacov/Desktop/university/ea191/bp_state_estimate/hmm_model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomyaacov/Desktop/university/ea191/bp_state_estimate/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0252A6-32BB-C148-8BBE-7BF7BB467B74}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EE0546-A891-0047-B7A3-7E78544F4028}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F5438FF8-32BD-8142-96DE-9EF2C2D3070E}"/>
   </bookViews>
@@ -454,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E28B8B0-7AD1-1B43-830C-9BDA3F2B5925}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,10 +495,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="C2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -510,10 +510,10 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="I2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -674,11 +674,11 @@
       </c>
       <c r="B8">
         <f>$B2*H2</f>
-        <v>0.55999999999999994</v>
+        <v>0.72000000000000008</v>
       </c>
       <c r="C8">
         <f t="shared" ref="C8:E8" si="0">$B2*I2</f>
-        <v>0.13999999999999999</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -690,11 +690,11 @@
       </c>
       <c r="F8">
         <f>$C2*H2</f>
-        <v>0.24</v>
+        <v>0.18000000000000002</v>
       </c>
       <c r="G8">
         <f t="shared" ref="G8:I8" si="1">$C2*I2</f>
-        <v>0.06</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
@@ -751,7 +751,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="4"/>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="E9">
         <f t="shared" si="4"/>
@@ -767,7 +767,7 @@
       </c>
       <c r="H9">
         <f t="shared" si="5"/>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="I9">
         <f t="shared" si="5"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="8"/>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="F10">
         <f>$C2*H4</f>
@@ -840,7 +840,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="9"/>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="J10">
         <f>$D2*H4</f>
@@ -881,7 +881,7 @@
       </c>
       <c r="B11">
         <f>$B2*H5</f>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="C11">
         <f t="shared" ref="C11:E11" si="12">$B2*I5</f>
@@ -897,7 +897,7 @@
       </c>
       <c r="F11">
         <f>$C2*H5</f>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:I11" si="13">$C2*I5</f>
@@ -982,11 +982,11 @@
       </c>
       <c r="J12">
         <f>$D3*H2</f>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="K12">
         <f t="shared" ref="K12:M12" si="18">$D3*I2</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="L12">
         <f t="shared" si="18"/>
@@ -1274,11 +1274,11 @@
       </c>
       <c r="N16">
         <f>$E4*H2</f>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="O16">
         <f t="shared" ref="O16:Q16" si="35">$E4*I2</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="P16">
         <f t="shared" si="35"/>
@@ -1502,11 +1502,11 @@
       </c>
       <c r="B20">
         <f>$B5*H2</f>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C20">
         <f t="shared" ref="C20:E20" si="48">$B5*I2</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D20">
         <f t="shared" si="48"/>

</xml_diff>